<commit_message>
Happy New 2016 year!
</commit_message>
<xml_diff>
--- a/Spr/xls_forms/FA.xlsx
+++ b/Spr/xls_forms/FA.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="480" yWindow="75" windowWidth="22710" windowHeight="10800"/>
   </bookViews>
   <sheets>
-    <sheet name="экспликация А" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="2" r:id="rId1"/>
+    <sheet name="экспликация А" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -303,7 +304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -398,6 +399,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -706,10 +708,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:EL1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:EL1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25"/>
+  <sheetData>
+    <row r="1" spans="1:142">
+      <c r="A1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="34"/>
+      <c r="X1" s="34"/>
+      <c r="Y1" s="34"/>
+      <c r="Z1" s="34"/>
+      <c r="AA1" s="34"/>
+      <c r="AB1" s="34"/>
+      <c r="AC1" s="34"/>
+      <c r="AD1" s="34"/>
+      <c r="AE1" s="34"/>
+      <c r="AF1" s="34"/>
+      <c r="AG1" s="34"/>
+      <c r="AH1" s="34"/>
+      <c r="AI1" s="34"/>
+      <c r="AJ1" s="34"/>
+      <c r="AK1" s="34"/>
+      <c r="AL1" s="34"/>
+      <c r="AM1" s="34"/>
+      <c r="AN1" s="34"/>
+      <c r="AO1" s="34"/>
+      <c r="AP1" s="34"/>
+      <c r="AQ1" s="34"/>
+      <c r="AR1" s="34"/>
+      <c r="AS1" s="34"/>
+      <c r="AT1" s="34"/>
+      <c r="AU1" s="34"/>
+      <c r="AV1" s="34"/>
+      <c r="AW1" s="34"/>
+      <c r="AX1" s="34"/>
+      <c r="AY1" s="34"/>
+      <c r="AZ1" s="34"/>
+      <c r="BA1" s="34"/>
+      <c r="BB1" s="34"/>
+      <c r="BC1" s="34"/>
+      <c r="BD1" s="34"/>
+      <c r="BE1" s="34"/>
+      <c r="BF1" s="34"/>
+      <c r="BG1" s="34"/>
+      <c r="BH1" s="34"/>
+      <c r="BI1" s="34"/>
+      <c r="BJ1" s="34"/>
+      <c r="BK1" s="34"/>
+      <c r="BL1" s="34"/>
+      <c r="BM1" s="34"/>
+      <c r="BN1" s="34"/>
+      <c r="BO1" s="34"/>
+      <c r="BP1" s="34"/>
+      <c r="BQ1" s="34"/>
+      <c r="BR1" s="34"/>
+      <c r="BS1" s="34"/>
+      <c r="BT1" s="34"/>
+      <c r="BU1" s="34"/>
+      <c r="BV1" s="34"/>
+      <c r="BW1" s="34"/>
+      <c r="BX1" s="34"/>
+      <c r="BY1" s="34"/>
+      <c r="BZ1" s="34"/>
+      <c r="CA1" s="34"/>
+      <c r="CB1" s="34"/>
+      <c r="CC1" s="34"/>
+      <c r="CD1" s="34"/>
+      <c r="CE1" s="34"/>
+      <c r="CF1" s="34"/>
+      <c r="CG1" s="34"/>
+      <c r="CH1" s="34"/>
+      <c r="CI1" s="34"/>
+      <c r="CJ1" s="34"/>
+      <c r="CK1" s="34"/>
+      <c r="CL1" s="34"/>
+      <c r="CM1" s="34"/>
+      <c r="CN1" s="34"/>
+      <c r="CO1" s="34"/>
+      <c r="CP1" s="34"/>
+      <c r="CQ1" s="34"/>
+      <c r="CR1" s="34"/>
+      <c r="CS1" s="34"/>
+      <c r="CT1" s="34"/>
+      <c r="CU1" s="34"/>
+      <c r="CV1" s="34"/>
+      <c r="CW1" s="34"/>
+      <c r="CX1" s="34"/>
+      <c r="CY1" s="34"/>
+      <c r="CZ1" s="34"/>
+      <c r="DA1" s="34"/>
+      <c r="DB1" s="34"/>
+      <c r="DC1" s="34"/>
+      <c r="DD1" s="34"/>
+      <c r="DE1" s="34"/>
+      <c r="DF1" s="34"/>
+      <c r="DG1" s="34"/>
+      <c r="DH1" s="34"/>
+      <c r="DI1" s="34"/>
+      <c r="DJ1" s="34"/>
+      <c r="DK1" s="34"/>
+      <c r="DL1" s="34"/>
+      <c r="DM1" s="34"/>
+      <c r="DN1" s="34"/>
+      <c r="DO1" s="34"/>
+      <c r="DP1" s="34"/>
+      <c r="DQ1" s="34"/>
+      <c r="DR1" s="34"/>
+      <c r="DS1" s="34"/>
+      <c r="DT1" s="34"/>
+      <c r="DU1" s="34"/>
+      <c r="DV1" s="34"/>
+      <c r="DW1" s="34"/>
+      <c r="DX1" s="34"/>
+      <c r="DY1" s="34"/>
+      <c r="DZ1" s="34"/>
+      <c r="EA1" s="34"/>
+      <c r="EB1" s="34"/>
+      <c r="EC1" s="34"/>
+      <c r="ED1" s="34"/>
+      <c r="EE1" s="34"/>
+      <c r="EF1" s="34"/>
+      <c r="EG1" s="34"/>
+      <c r="EH1" s="34"/>
+      <c r="EI1" s="34"/>
+      <c r="EJ1" s="34"/>
+      <c r="EK1" s="34"/>
+      <c r="EL1" s="34"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W25" sqref="W25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>

</xml_diff>

<commit_message>
fixed xls formula saving
</commit_message>
<xml_diff>
--- a/Spr/xls_forms/FA.xlsx
+++ b/Spr/xls_forms/FA.xlsx
@@ -18,7 +18,7 @@
     <definedName name="ExpB_24_04_2015_11_47">#REF!</definedName>
     <definedName name="ExpFormaB_Work">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -940,9 +940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16:BM28"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2592,8 +2590,6 @@
     <row r="40" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="W12:W14"/>
-    <mergeCell ref="U13:U14"/>
     <mergeCell ref="V13:V14"/>
     <mergeCell ref="A10:U10"/>
     <mergeCell ref="A11:U11"/>
@@ -2608,32 +2604,27 @@
     <mergeCell ref="N12:N14"/>
     <mergeCell ref="O12:R12"/>
     <mergeCell ref="S12:S14"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="AJ12:AK12"/>
+    <mergeCell ref="AL12:AL14"/>
+    <mergeCell ref="AM12:AO12"/>
+    <mergeCell ref="AH12:AH14"/>
+    <mergeCell ref="AI12:AI14"/>
+    <mergeCell ref="AF13:AF14"/>
+    <mergeCell ref="AG13:AG14"/>
     <mergeCell ref="T12:T14"/>
     <mergeCell ref="U12:V12"/>
     <mergeCell ref="Z12:AB12"/>
     <mergeCell ref="AC12:AC14"/>
     <mergeCell ref="AD12:AG12"/>
-    <mergeCell ref="AH12:AH14"/>
-    <mergeCell ref="AI12:AI14"/>
-    <mergeCell ref="AF13:AF14"/>
-    <mergeCell ref="AG13:AG14"/>
-    <mergeCell ref="AU12:AY12"/>
-    <mergeCell ref="AZ12:AZ14"/>
-    <mergeCell ref="BA12:BM12"/>
+    <mergeCell ref="W12:W14"/>
+    <mergeCell ref="U13:U14"/>
     <mergeCell ref="J13:J14"/>
     <mergeCell ref="K13:K14"/>
     <mergeCell ref="L13:L14"/>
     <mergeCell ref="M13:M14"/>
     <mergeCell ref="O13:O14"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="AJ12:AK12"/>
-    <mergeCell ref="AL12:AL14"/>
-    <mergeCell ref="AM12:AO12"/>
-    <mergeCell ref="AP12:AP14"/>
-    <mergeCell ref="AQ12:AS12"/>
-    <mergeCell ref="AT12:AT14"/>
-    <mergeCell ref="BB13:BC13"/>
     <mergeCell ref="BD13:BD14"/>
     <mergeCell ref="AO13:AO14"/>
     <mergeCell ref="AQ13:AQ14"/>
@@ -2641,6 +2632,13 @@
     <mergeCell ref="AS13:AS14"/>
     <mergeCell ref="AU13:AU14"/>
     <mergeCell ref="AV13:AV14"/>
+    <mergeCell ref="AZ12:AZ14"/>
+    <mergeCell ref="BA12:BM12"/>
+    <mergeCell ref="AP12:AP14"/>
+    <mergeCell ref="AQ12:AS12"/>
+    <mergeCell ref="AT12:AT14"/>
+    <mergeCell ref="BB13:BC13"/>
+    <mergeCell ref="AU12:AY12"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="AW13:AW14"/>
     <mergeCell ref="AX13:AX14"/>

</xml_diff>